<commit_message>
codes used for first draft of paper
</commit_message>
<xml_diff>
--- a/document/performance_analysis_comparison.xlsx
+++ b/document/performance_analysis_comparison.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Praveen\PostDoc@SIT\SIT2024\MI_TimeAttention\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A5E92C-A107-41EE-88FC-914F55BD9E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BD931D-8BEE-4AE1-A413-019C303E21C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1665" windowWidth="29040" windowHeight="15720" xr2:uid="{895801F1-468B-47CF-B391-CABAF5D217E3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{895801F1-468B-47CF-B391-CABAF5D217E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
   <si>
     <t>SubID</t>
   </si>
@@ -137,12 +138,84 @@
 Sample Scale
 Dense</t>
   </si>
+  <si>
+    <t>Subject Specific 
+Sample Scale
+Electrode Scale
+Dense</t>
+  </si>
+  <si>
+    <t>batch_size=16
+learning_rate=1e-4
+min_epochs = 50
+best_val_acc = 70.00
+num_epochs = 500
+patience = 5  
+min_delta = 1e-4 
+el_scaler_red_rate = 2
+sample_scaler_red_rate = 4</t>
+  </si>
+  <si>
+    <t>lr=1e-3</t>
+  </si>
+  <si>
+    <t>Subject Specific
+Dense</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">batch_size=16
+learning_rate=1e-3
+min_epochs = 5
+best_val_acc = 75
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>num_epochs = 20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+patience = 5  
+min_delta = 1e-3 
+el_scaler_red_rate = 2
+sample_scaler_red_rate = 4</t>
+    </r>
+  </si>
+  <si>
+    <t>subIDs</t>
+  </si>
+  <si>
+    <t>Electrode Scaling</t>
+  </si>
+  <si>
+    <t>Sample Scaling</t>
+  </si>
+  <si>
+    <t>Both Scaling</t>
+  </si>
+  <si>
+    <t>W-PLV</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +241,13 @@
       <sz val="8"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -196,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -211,16 +291,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -236,6 +314,1313 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.786480822961646E-2"/>
+          <c:y val="3.3152501506931886E-2"/>
+          <c:w val="0.93869433155532966"/>
+          <c:h val="0.91224150778621027"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$2:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>S01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>S02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>S03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>S04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>S05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>S06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>S07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>S08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>S09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>S10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>S11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>S12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>S13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>S14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$2:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>54.17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52.08</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.58</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60.42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>66.67</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58.33</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>52.08</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>56.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>58.33</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60.42</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>68.75</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60.42</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>54.17</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>66.67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2E81-4C93-866F-2FA4BF0D4CCB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$2:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>S01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>S02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>S03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>S04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>S05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>S06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>S07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>S08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>S09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>S10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>S11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>S12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>S13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>S14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$C$2:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>71.111111109999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72.888888890000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>73.111111109999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75.111111109999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65.111111109999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55.111111110000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>69.333333330000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>58.222222219999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>56.888888889999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>62.888888889999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>52.222222219999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>62.444444439999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65.111111109999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2E81-4C93-866F-2FA4BF0D4CCB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$2:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>S01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>S02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>S03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>S04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>S05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>S06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>S07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>S08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>S09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>S10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>S11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>S12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>S13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>S14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$D$2:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>66.888888890000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>69.111111109999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73.333333330000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62.666666669999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68.666666669999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>62.222222219999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>56.444444439999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>67.111111109999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>69.111111109999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>68.888888890000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>52.444444439999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2E81-4C93-866F-2FA4BF0D4CCB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$2:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>S01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>S02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>S03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>S04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>S05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>S06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>S07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>S08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>S09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>S10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>S11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>S12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>S13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>S14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$E$2:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67.333333330000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79.111111109999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74.888888890000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>73.555555560000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>79.555555560000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>54.222222219999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>75.333333330000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>56.222222219999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>58.222222219999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>54.888888889999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70.666666669999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>48.222222219999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>75.555555560000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2E81-4C93-866F-2FA4BF0D4CCB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="621809023"/>
+        <c:axId val="621809503"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="621809023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="621809503"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="621809503"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="621809023"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.67525915989331975"/>
+          <c:y val="0.13817995851784351"/>
+          <c:w val="0.29755625724449419"/>
+          <c:h val="4.7831967432642356E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{550EC5C9-4553-0737-5F18-2F0E5FF085BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -557,48 +1942,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9216A6BF-7C7C-4A9F-88A0-3B53B3C3430B}">
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" customWidth="1"/>
+    <col min="7" max="7" width="6.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" customWidth="1"/>
-    <col min="12" max="12" width="25.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" customWidth="1"/>
+    <col min="12" max="12" width="25.44140625" customWidth="1"/>
     <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-    </row>
-    <row r="3" spans="1:20" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+    </row>
+    <row r="3" spans="1:20" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -611,8 +1996,11 @@
       <c r="E3" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F3" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -625,75 +2013,98 @@
       <c r="D4">
         <v>66.66</v>
       </c>
-      <c r="E4" s="10"/>
-    </row>
-    <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>56.22</v>
+      </c>
+      <c r="F4">
+        <v>68.44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2">
         <v>52.08</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>63.11</v>
       </c>
       <c r="D5">
         <v>54.22</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
+      <c r="E5">
+        <v>56.88</v>
+      </c>
+      <c r="F5">
+        <v>38.22</v>
+      </c>
+      <c r="G5">
+        <v>58</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
       <c r="S5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="2">
         <v>64.58</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>64.22</v>
       </c>
       <c r="D6">
         <v>62.22</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
+      <c r="E6">
+        <v>64</v>
+      </c>
+      <c r="F6">
+        <v>70.66</v>
+      </c>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
       <c r="R6" s="5"/>
       <c r="S6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="T6" s="4"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="2">
         <v>60.42</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>62.22</v>
       </c>
       <c r="D7">
         <v>58.22</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
+      <c r="E7">
+        <v>60.22</v>
+      </c>
+      <c r="F7">
+        <v>64.88</v>
+      </c>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
       <c r="P7" s="1"/>
       <c r="R7" s="4"/>
       <c r="S7" s="4" t="s">
@@ -701,249 +2112,301 @@
       </c>
       <c r="T7" s="4"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="2">
         <v>66.67</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>58.66</v>
       </c>
       <c r="D8">
         <v>58.44</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
+      <c r="E8">
+        <v>52.22</v>
+      </c>
+      <c r="F8">
+        <v>73.11</v>
+      </c>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="T8" s="4"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="2">
         <v>58.33</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>60.22</v>
       </c>
       <c r="D9">
         <v>56.22</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
+      <c r="E9">
+        <v>60.44</v>
+      </c>
+      <c r="F9">
+        <v>62.88</v>
+      </c>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
       <c r="R9" s="4"/>
       <c r="S9" s="4" t="s">
         <v>20</v>
       </c>
       <c r="T9" s="4"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="2">
         <v>52.08</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>42</v>
       </c>
       <c r="D10">
         <v>52.44</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
+      <c r="E10">
+        <v>33.33</v>
+      </c>
+      <c r="F10">
+        <v>50.22</v>
+      </c>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
       <c r="R10" s="4"/>
       <c r="S10" s="4" t="s">
         <v>21</v>
       </c>
       <c r="T10" s="4"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="2">
         <v>56.25</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>65.33</v>
       </c>
       <c r="D11">
         <v>67.11</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
+      <c r="E11">
+        <v>69.11</v>
+      </c>
+      <c r="F11">
+        <v>69.11</v>
+      </c>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
       <c r="R11" s="4"/>
       <c r="S11" s="4" t="s">
         <v>22</v>
       </c>
       <c r="T11" s="4"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="2">
         <v>58.33</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>64.66</v>
       </c>
       <c r="D12">
         <v>67.11</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
+      <c r="E12">
+        <v>66.66</v>
+      </c>
+      <c r="F12">
+        <v>55.55</v>
+      </c>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
       <c r="R12" s="4"/>
       <c r="S12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="T12" s="4"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="2">
         <v>60.42</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>50.88</v>
       </c>
       <c r="D13">
         <v>68.66</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
+      <c r="E13">
+        <v>56.66</v>
+      </c>
+      <c r="F13">
+        <v>59.33</v>
+      </c>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
       <c r="R13" s="4"/>
       <c r="S13" s="4" t="s">
         <v>24</v>
       </c>
       <c r="T13" s="4"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="2">
         <v>68.75</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>56.667000000000002</v>
       </c>
       <c r="D14">
         <v>60.44</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
+      <c r="E14">
+        <v>48.44</v>
+      </c>
+      <c r="F14">
+        <v>64.88</v>
+      </c>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="2">
         <v>60.42</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <v>51.55</v>
       </c>
       <c r="D15">
         <v>47.77</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>52.44</v>
+      </c>
+      <c r="F15">
+        <v>64.88</v>
+      </c>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="2">
         <v>54.17</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <v>66.88</v>
       </c>
       <c r="D16">
         <v>64.88</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>66.22</v>
+      </c>
+      <c r="F16">
+        <v>37.11</v>
+      </c>
+      <c r="G16">
+        <v>57.77</v>
+      </c>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="2">
         <v>66.67</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="8">
         <v>69.11</v>
       </c>
       <c r="D17">
         <v>61.11</v>
       </c>
-      <c r="E17" s="10"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C18" s="9"/>
-      <c r="E18" s="10"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>54.44</v>
+      </c>
+      <c r="F17">
+        <v>56.44</v>
+      </c>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f>AVERAGE(B4:B17)</f>
         <v>59.524285714285703</v>
@@ -956,45 +2419,54 @@
         <f>AVERAGE(D4:D17)</f>
         <v>60.392857142857146</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="1"/>
+      <c r="E19" s="1">
+        <f>AVERAGE(E4:E17)</f>
+        <v>56.948571428571427</v>
+      </c>
+      <c r="F19" s="1">
+        <f>AVERAGE(F4:F17)</f>
+        <v>59.693571428571431</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E20" s="10"/>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:15" ht="165" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="168.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
+      <c r="F21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="I21" s="5"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I27" s="4"/>
     </row>
   </sheetData>
@@ -1004,4 +2476,606 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA27AEA-8ACF-464D-B31A-A6456E514866}">
+  <dimension ref="A2:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>54.17</v>
+      </c>
+      <c r="C3">
+        <v>64.44</v>
+      </c>
+      <c r="D3">
+        <v>66.88</v>
+      </c>
+      <c r="E3">
+        <v>66.66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>52.08</v>
+      </c>
+      <c r="C4" s="8">
+        <v>56.88</v>
+      </c>
+      <c r="D4">
+        <v>64.88</v>
+      </c>
+      <c r="E4">
+        <v>69.77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>64.58</v>
+      </c>
+      <c r="C5" s="8">
+        <v>79.11</v>
+      </c>
+      <c r="D5">
+        <v>78.66</v>
+      </c>
+      <c r="E5">
+        <v>69.11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>60.42</v>
+      </c>
+      <c r="C6" s="8">
+        <v>64.66</v>
+      </c>
+      <c r="D6">
+        <v>66.44</v>
+      </c>
+      <c r="E6">
+        <v>77.55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>66.67</v>
+      </c>
+      <c r="C7" s="8">
+        <v>68.88</v>
+      </c>
+      <c r="D7">
+        <v>58.44</v>
+      </c>
+      <c r="E7">
+        <v>69.33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>58.33</v>
+      </c>
+      <c r="C8" s="8">
+        <v>56.44</v>
+      </c>
+      <c r="D8">
+        <v>71.11</v>
+      </c>
+      <c r="E8">
+        <v>56.44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>52.08</v>
+      </c>
+      <c r="C9" s="8">
+        <v>58.44</v>
+      </c>
+      <c r="D9">
+        <v>36</v>
+      </c>
+      <c r="E9">
+        <v>48.66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>56.25</v>
+      </c>
+      <c r="C10" s="8">
+        <v>75.77</v>
+      </c>
+      <c r="D10">
+        <v>73.77</v>
+      </c>
+      <c r="E10">
+        <v>75.77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>58.33</v>
+      </c>
+      <c r="C11" s="8">
+        <v>67.77</v>
+      </c>
+      <c r="D11">
+        <v>60.44</v>
+      </c>
+      <c r="E11">
+        <v>65.33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>60.42</v>
+      </c>
+      <c r="C12" s="8">
+        <v>63.11</v>
+      </c>
+      <c r="D12">
+        <v>60.22</v>
+      </c>
+      <c r="E12">
+        <v>58.66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>68.75</v>
+      </c>
+      <c r="C13" s="8">
+        <v>62.66</v>
+      </c>
+      <c r="D13">
+        <v>63.33</v>
+      </c>
+      <c r="E13">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>60.42</v>
+      </c>
+      <c r="C14" s="8">
+        <v>58.4</v>
+      </c>
+      <c r="D14">
+        <v>66.44</v>
+      </c>
+      <c r="E14">
+        <v>72.66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <v>54.17</v>
+      </c>
+      <c r="C15" s="8">
+        <v>50</v>
+      </c>
+      <c r="D15">
+        <v>68.44</v>
+      </c>
+      <c r="E15">
+        <v>62.66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <v>66.67</v>
+      </c>
+      <c r="C16" s="8">
+        <v>62.88</v>
+      </c>
+      <c r="D16">
+        <v>69.66</v>
+      </c>
+      <c r="E16">
+        <v>73.55</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="3">
+        <f>AVERAGE(B3:B16)</f>
+        <v>59.524285714285703</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" ref="C18:E18" si="0">AVERAGE(C3:C16)</f>
+        <v>63.53142857142857</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>64.622142857142862</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>65.867857142857133</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="C20" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA35073A-5886-427B-B323-A29D1511D988}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>54.17</v>
+      </c>
+      <c r="C2">
+        <v>71.111111109999996</v>
+      </c>
+      <c r="D2">
+        <v>66.888888890000004</v>
+      </c>
+      <c r="E2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>52.08</v>
+      </c>
+      <c r="C3">
+        <v>86</v>
+      </c>
+      <c r="D3">
+        <v>69.111111109999996</v>
+      </c>
+      <c r="E3">
+        <v>67.333333330000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>64.58</v>
+      </c>
+      <c r="C4">
+        <v>72.888888890000004</v>
+      </c>
+      <c r="D4">
+        <v>73.333333330000002</v>
+      </c>
+      <c r="E4">
+        <v>79.111111109999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>60.42</v>
+      </c>
+      <c r="C5">
+        <v>73.111111109999996</v>
+      </c>
+      <c r="D5">
+        <v>62.666666669999998</v>
+      </c>
+      <c r="E5">
+        <v>74.888888890000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>66.67</v>
+      </c>
+      <c r="C6">
+        <v>75.111111109999996</v>
+      </c>
+      <c r="D6">
+        <v>68.666666669999998</v>
+      </c>
+      <c r="E6">
+        <v>73.555555560000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>58.33</v>
+      </c>
+      <c r="C7">
+        <v>65.111111109999996</v>
+      </c>
+      <c r="D7">
+        <v>62.222222219999999</v>
+      </c>
+      <c r="E7">
+        <v>79.555555560000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>52.08</v>
+      </c>
+      <c r="C8">
+        <v>55.111111110000003</v>
+      </c>
+      <c r="D8">
+        <v>46</v>
+      </c>
+      <c r="E8">
+        <v>54.222222219999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>56.25</v>
+      </c>
+      <c r="C9">
+        <v>69.333333330000002</v>
+      </c>
+      <c r="D9">
+        <v>78</v>
+      </c>
+      <c r="E9">
+        <v>75.333333330000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>58.33</v>
+      </c>
+      <c r="C10">
+        <v>58.222222219999999</v>
+      </c>
+      <c r="D10">
+        <v>56</v>
+      </c>
+      <c r="E10">
+        <v>56.222222219999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>60.42</v>
+      </c>
+      <c r="C11">
+        <v>56.888888889999997</v>
+      </c>
+      <c r="D11">
+        <v>56.444444439999998</v>
+      </c>
+      <c r="E11">
+        <v>58.222222219999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>68.75</v>
+      </c>
+      <c r="C12">
+        <v>62.888888889999997</v>
+      </c>
+      <c r="D12">
+        <v>67.111111109999996</v>
+      </c>
+      <c r="E12">
+        <v>54.888888889999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>60.42</v>
+      </c>
+      <c r="C13">
+        <v>52.222222219999999</v>
+      </c>
+      <c r="D13">
+        <v>69.111111109999996</v>
+      </c>
+      <c r="E13">
+        <v>70.666666669999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>54.17</v>
+      </c>
+      <c r="C14">
+        <v>62.444444439999998</v>
+      </c>
+      <c r="D14">
+        <v>68.888888890000004</v>
+      </c>
+      <c r="E14">
+        <v>48.222222219999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>66.67</v>
+      </c>
+      <c r="C15">
+        <v>65.111111109999996</v>
+      </c>
+      <c r="D15">
+        <v>52.444444439999998</v>
+      </c>
+      <c r="E15">
+        <v>75.555555560000002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <f>AVERAGE(B2:B15)</f>
+        <v>59.524285714285703</v>
+      </c>
+      <c r="C17">
+        <v>66.111111109999996</v>
+      </c>
+      <c r="D17">
+        <v>64.063492060000002</v>
+      </c>
+      <c r="E17">
+        <v>65.984126979999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <f>_xlfn.STDEV.S(B2:B15)</f>
+        <v>5.5258034073520292</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:E18" si="0">_xlfn.STDEV.S(C2:C15)</f>
+        <v>9.1731264473394116</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>8.6937680893464897</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>10.841678325181135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated documents with SMC2025
</commit_message>
<xml_diff>
--- a/document/performance_analysis_comparison.xlsx
+++ b/document/performance_analysis_comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Praveen\PostDoc@SIT\SIT2024\MI_TimeAttention\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BD931D-8BEE-4AE1-A413-019C303E21C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57844F43-32B0-4B7C-8D75-F3CB378A5641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{895801F1-468B-47CF-B391-CABAF5D217E3}"/>
+    <workbookView xWindow="28695" yWindow="-1545" windowWidth="11520" windowHeight="15585" activeTab="2" xr2:uid="{895801F1-468B-47CF-B391-CABAF5D217E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
   <si>
     <t>SubID</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>W-PLV</t>
+  </si>
+  <si>
+    <t>EEGNet</t>
   </si>
 </sst>
 </file>
@@ -250,7 +253,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,8 +266,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -272,11 +281,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -296,6 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1586,16 +1611,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1966,22 +1991,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
     </row>
     <row r="3" spans="1:20" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -2778,15 +2803,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA35073A-5886-427B-B323-A29D1511D988}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -2802,8 +2833,11 @@
       <c r="E1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2819,8 +2853,11 @@
       <c r="E2">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2836,8 +2873,11 @@
       <c r="E3">
         <v>67.333333330000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="9">
+        <v>52.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2853,8 +2893,11 @@
       <c r="E4">
         <v>79.111111109999996</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="9">
+        <v>54.17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2870,8 +2913,11 @@
       <c r="E5">
         <v>74.888888890000004</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2887,8 +2933,11 @@
       <c r="E6">
         <v>73.555555560000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2904,8 +2953,11 @@
       <c r="E7">
         <v>79.555555560000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2921,8 +2973,11 @@
       <c r="E8">
         <v>54.222222219999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="9">
+        <v>58.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2938,8 +2993,11 @@
       <c r="E9">
         <v>75.333333330000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="9">
+        <v>54.17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2955,8 +3013,11 @@
       <c r="E10">
         <v>56.222222219999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="9">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2972,8 +3033,11 @@
       <c r="E11">
         <v>58.222222219999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" s="9">
+        <v>52.08</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2989,8 +3053,11 @@
       <c r="E12">
         <v>54.888888889999997</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3006,8 +3073,11 @@
       <c r="E13">
         <v>70.666666669999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" s="9">
+        <v>39.58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -3023,8 +3093,11 @@
       <c r="E14">
         <v>48.222222219999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="9">
+        <v>52.08</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -3040,38 +3113,66 @@
       <c r="E15">
         <v>75.555555560000002</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="9">
+        <v>45.83</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17">
         <f>AVERAGE(B2:B15)</f>
         <v>59.524285714285703</v>
       </c>
       <c r="C17">
-        <v>66.111111109999996</v>
+        <f t="shared" ref="C17:E17" si="0">AVERAGE(C2:C15)</f>
+        <v>66.11111111000001</v>
       </c>
       <c r="D17">
-        <v>64.063492060000002</v>
+        <f t="shared" si="0"/>
+        <v>64.063492062857136</v>
       </c>
       <c r="E17">
-        <v>65.984126979999999</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>65.984126984285723</v>
+      </c>
+      <c r="F17">
+        <f>AVERAGE(F2:F15)</f>
+        <v>51.487142857142871</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18">
         <f>_xlfn.STDEV.S(B2:B15)</f>
         <v>5.5258034073520292</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="C18:E18" si="0">_xlfn.STDEV.S(C2:C15)</f>
+        <f t="shared" ref="C18:E18" si="1">_xlfn.STDEV.S(C2:C15)</f>
         <v>9.1731264473394116</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.6937680893464897</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10.841678325181135</v>
+      </c>
+      <c r="F18">
+        <f>_xlfn.STDEV.S(F2:F15)</f>
+        <v>5.3233801126892892</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <f>AVERAGE(C4:C15)</f>
+        <v>64.037037035833336</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="D20:E20" si="2">AVERAGE(D4:D15)</f>
+        <v>63.407407406666664</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>66.703703704166671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>